<commit_message>
GeoSpatial v3. Adding crime data
</commit_message>
<xml_diff>
--- a/data_processed/data_dictionary/data_dictionary_v2.xlsx
+++ b/data_processed/data_dictionary/data_dictionary_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shennalu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Antigravity/Airbnb-Renting-Optimizer/data_processed/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77B8830D-B9C1-AC40-BDA3-E4183CCA13DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D2A35C-C483-0C4D-AE90-59A78BB55B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="28040" windowHeight="16260" activeTab="2" xr2:uid="{0EA26DC6-FC12-1B47-82F1-A6338E56EE2B}"/>
+    <workbookView xWindow="-4300" yWindow="-17680" windowWidth="25600" windowHeight="16060" activeTab="2" xr2:uid="{0EA26DC6-FC12-1B47-82F1-A6338E56EE2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Identifier" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
   <si>
     <t>feature_name</t>
   </si>
@@ -227,6 +227,87 @@
   </si>
   <si>
     <t>winter_occupancy_proxy</t>
+  </si>
+  <si>
+    <t>dist_navy_pier_miles</t>
+  </si>
+  <si>
+    <t>haversine_dist(listing, navy_pier)</t>
+  </si>
+  <si>
+    <t>Straight-line distance to Navy Pier in miles</t>
+  </si>
+  <si>
+    <t>is_landmark_proximate</t>
+  </si>
+  <si>
+    <t>(dist_to_landmarks &lt;= 1.0mi).astype(int)</t>
+  </si>
+  <si>
+    <t>Binary flag for listings within 1 mile of major Chicago landmarks</t>
+  </si>
+  <si>
+    <t>transit_north_premium</t>
+  </si>
+  <si>
+    <t>(1 / (dist_navy_pier + 1)) * lat_norm</t>
+  </si>
+  <si>
+    <t>Interaction between landmark proximity and North Side latitude</t>
+  </si>
+  <si>
+    <t>is_premium_transit_hub</t>
+  </si>
+  <si>
+    <t>is_rail_accessible * lat_norm</t>
+  </si>
+  <si>
+    <t>Weighted score for rail access (within 0.5mi) scaled by North Side prestige</t>
+  </si>
+  <si>
+    <t>shoreline_gravity</t>
+  </si>
+  <si>
+    <t>1 / (dist_to_shoreline**2 + 1)</t>
+  </si>
+  <si>
+    <t>Exponentially decaying score based on distance to Lake Michigan</t>
+  </si>
+  <si>
+    <t>dist_to_beach_miles</t>
+  </si>
+  <si>
+    <t>min(dist_to_all_public_beaches)</t>
+  </si>
+  <si>
+    <t>Distance to the nearest public beach access point</t>
+  </si>
+  <si>
+    <t>crime_density_total</t>
+  </si>
+  <si>
+    <t>Crimes (Chicago Data Portal)</t>
+  </si>
+  <si>
+    <t>count(crimes) / area_sq_miles</t>
+  </si>
+  <si>
+    <t>Neighborhood-level crime incidents per square mile</t>
+  </si>
+  <si>
+    <t>nb_homicides_half_mile</t>
+  </si>
+  <si>
+    <t>count(homicides within 0.5mi buffer)</t>
+  </si>
+  <si>
+    <t>Localized count of homicides within walking distance</t>
+  </si>
+  <si>
+    <t>listings.csv, Chicago Data Portal</t>
+  </si>
+  <si>
+    <t>listings.csv, CTA, Metra</t>
   </si>
 </sst>
 </file>
@@ -302,9 +383,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -342,7 +423,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -448,7 +529,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -590,7 +671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -852,16 +933,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E594965-D0BA-924D-88FE-5C095C8246D7}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
@@ -1064,7 +1145,168 @@
         <v>14</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>